<commit_message>
Fixed minor issues(pincode, ll no.) in form validation
</commit_message>
<xml_diff>
--- a/IndianCitiesDb.xlsx
+++ b/IndianCitiesDb.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SanikaChepe\rasa_projects\rasabot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SanikaChepe\rasa_projects\ai-based-chatbot-final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD3A8D2C-73FF-4196-9DAB-3259BC5132C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0097E245-1091-470A-B3E5-401F7BD417D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="248">
   <si>
     <t>City</t>
   </si>
@@ -766,6 +766,9 @@
   </si>
   <si>
     <t>Nashik</t>
+  </si>
+  <si>
+    <t>Nagpur</t>
   </si>
 </sst>
 </file>
@@ -1115,10 +1118,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B214"/>
+  <dimension ref="A1:B215"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A129" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="A141" sqref="A141"/>
+      <selection activeCell="F141" sqref="F141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2266,63 +2269,63 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>169</v>
+        <v>247</v>
       </c>
       <c r="B143" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B144" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B145" t="s">
-        <v>5</v>
+        <v>82</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B146" t="s">
-        <v>73</v>
+        <v>5</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B147" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B148" t="s">
-        <v>175</v>
+        <v>17</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B149" t="s">
-        <v>27</v>
+        <v>175</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B150" t="s">
         <v>27</v>
@@ -2330,23 +2333,23 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B151" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B152" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B153" t="s">
         <v>3</v>
@@ -2354,175 +2357,175 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B154" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B155" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B156" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B157" t="s">
-        <v>185</v>
+        <v>13</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B158" t="s">
-        <v>73</v>
+        <v>185</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B159" t="s">
-        <v>187</v>
+        <v>73</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B160" t="s">
-        <v>11</v>
+        <v>187</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B161" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B162" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B163" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B164" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B165" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B166" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B167" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B168" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B169" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B170" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B171" t="s">
-        <v>54</v>
+        <v>84</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B172" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B173" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B174" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B175" t="s">
         <v>9</v>
@@ -2530,119 +2533,119 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B176" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B177" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B178" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B179" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B180" t="s">
-        <v>54</v>
+        <v>11</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B181" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B182" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B183" t="s">
-        <v>212</v>
+        <v>23</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B184" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B185" t="s">
-        <v>40</v>
+        <v>214</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B186" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B187" t="s">
-        <v>86</v>
+        <v>17</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B188" t="s">
-        <v>219</v>
+        <v>86</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B189" t="s">
-        <v>27</v>
+        <v>219</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B190" t="s">
         <v>27</v>
@@ -2650,63 +2653,63 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B191" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B192" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B193" t="s">
-        <v>86</v>
+        <v>13</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B194" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B195" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B196" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B197" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B198" t="s">
         <v>70</v>
@@ -2714,95 +2717,95 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B199" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B200" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B201" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B202" t="s">
-        <v>70</v>
+        <v>17</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B203" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B204" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B205" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B206" t="s">
-        <v>70</v>
+        <v>13</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B207" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B208" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B209" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B210" t="s">
         <v>73</v>
@@ -2810,33 +2813,41 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B211" t="s">
-        <v>5</v>
+        <v>73</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B212" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B213" t="s">
-        <v>56</v>
+        <v>84</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
+        <v>244</v>
+      </c>
+      <c r="B214" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
         <v>245</v>
       </c>
-      <c r="B214" t="s">
+      <c r="B215" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>